<commit_message>
HW 3 error fixes
</commit_message>
<xml_diff>
--- a/Homework/Lesson 03 Homework - LP3/data/transp_prob3.xlsx
+++ b/Homework/Lesson 03 Homework - LP3/data/transp_prob3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Gdrive_snap_May_15/MS Data Science/DS 775/DS775_v2.0/Development _Version/C - Lesson 03 - LP 3/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Gdrive_snap_May_15/MS Data Science/DS 775/DS775_v2.0/Release_Version/Lesson 03 Homework - LP3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFF6B56-6B13-844C-9344-84014474E7CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880F5C1D-8498-C54B-A498-8E662F4060B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="1660" windowWidth="28800" windowHeight="16240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-39720" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tuples" sheetId="4" r:id="rId1"/>
@@ -692,15 +692,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y202"/>
+  <dimension ref="A1:W202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="X1" sqref="X1:X1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -725,11 +725,11 @@
       <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c r="V1" t="s">
+      <c r="U1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -778,17 +778,17 @@
       <c r="S2" t="s">
         <v>4</v>
       </c>
+      <c r="U2" t="s">
+        <v>0</v>
+      </c>
       <c r="V2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="W2" t="s">
-        <v>26</v>
-      </c>
-      <c r="X2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -834,17 +834,17 @@
       <c r="S3">
         <v>700</v>
       </c>
+      <c r="U3" t="s">
+        <v>20</v>
+      </c>
       <c r="V3" t="s">
-        <v>20</v>
-      </c>
-      <c r="W3" t="s">
         <v>15</v>
       </c>
-      <c r="X3">
+      <c r="W3">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -893,17 +893,17 @@
       <c r="S4">
         <v>560</v>
       </c>
+      <c r="U4" t="s">
+        <v>20</v>
+      </c>
       <c r="V4" t="s">
-        <v>20</v>
-      </c>
-      <c r="W4" t="s">
         <v>16</v>
       </c>
-      <c r="X4">
+      <c r="W4">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -952,21 +952,17 @@
       <c r="S5">
         <v>800</v>
       </c>
-      <c r="T5">
-        <f>SUM(S3:S5)</f>
-        <v>2060</v>
+      <c r="U5" t="s">
+        <v>20</v>
       </c>
       <c r="V5" t="s">
-        <v>20</v>
-      </c>
-      <c r="W5" t="s">
         <v>17</v>
       </c>
-      <c r="X5">
+      <c r="W5">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1012,17 +1008,17 @@
       <c r="S6">
         <v>500</v>
       </c>
+      <c r="U6" t="s">
+        <v>20</v>
+      </c>
       <c r="V6" t="s">
-        <v>20</v>
-      </c>
-      <c r="W6" t="s">
         <v>18</v>
       </c>
-      <c r="X6">
+      <c r="W6">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>37</v>
       </c>
@@ -1065,17 +1061,17 @@
       <c r="S7">
         <v>1000</v>
       </c>
+      <c r="U7" t="s">
+        <v>20</v>
+      </c>
       <c r="V7" t="s">
-        <v>20</v>
-      </c>
-      <c r="W7" t="s">
         <v>19</v>
       </c>
-      <c r="X7">
+      <c r="W7">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>38</v>
       </c>
@@ -1118,21 +1114,17 @@
       <c r="S8">
         <v>600</v>
       </c>
-      <c r="T8">
-        <f>SUM(S6:S8)</f>
-        <v>2100</v>
+      <c r="U8" t="s">
+        <v>20</v>
       </c>
       <c r="V8" t="s">
-        <v>20</v>
-      </c>
-      <c r="W8" t="s">
         <v>42</v>
       </c>
-      <c r="X8">
+      <c r="W8">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>39</v>
       </c>
@@ -1172,17 +1164,17 @@
       <c r="S9">
         <v>400</v>
       </c>
+      <c r="U9" t="s">
+        <v>20</v>
+      </c>
       <c r="V9" t="s">
-        <v>20</v>
-      </c>
-      <c r="W9" t="s">
         <v>43</v>
       </c>
-      <c r="X9">
+      <c r="W9">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>40</v>
       </c>
@@ -1222,21 +1214,17 @@
       <c r="S10">
         <v>670</v>
       </c>
-      <c r="T10">
-        <f>SUM(S9:S10)</f>
-        <v>1070</v>
+      <c r="U10" t="s">
+        <v>20</v>
       </c>
       <c r="V10" t="s">
-        <v>20</v>
-      </c>
-      <c r="W10" t="s">
         <v>44</v>
       </c>
-      <c r="X10">
+      <c r="W10">
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>41</v>
       </c>
@@ -1276,17 +1264,17 @@
       <c r="S11">
         <v>300</v>
       </c>
+      <c r="U11" t="s">
+        <v>20</v>
+      </c>
       <c r="V11" t="s">
-        <v>20</v>
-      </c>
-      <c r="W11" t="s">
         <v>45</v>
       </c>
-      <c r="X11">
+      <c r="W11">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>46</v>
       </c>
@@ -1323,21 +1311,17 @@
       <c r="S12">
         <v>280</v>
       </c>
-      <c r="T12">
-        <f>SUM(S11:S12)</f>
-        <v>580</v>
+      <c r="U12" t="s">
+        <v>20</v>
       </c>
       <c r="V12" t="s">
-        <v>20</v>
-      </c>
-      <c r="W12" t="s">
         <v>47</v>
       </c>
-      <c r="X12">
+      <c r="W12">
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>48</v>
       </c>
@@ -1374,17 +1358,17 @@
       <c r="S13">
         <v>1400</v>
       </c>
+      <c r="U13" t="s">
+        <v>20</v>
+      </c>
       <c r="V13" t="s">
-        <v>20</v>
-      </c>
-      <c r="W13" t="s">
         <v>46</v>
       </c>
-      <c r="X13">
+      <c r="W13">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>49</v>
       </c>
@@ -1421,17 +1405,17 @@
       <c r="S14">
         <v>1000</v>
       </c>
+      <c r="U14" t="s">
+        <v>20</v>
+      </c>
       <c r="V14" t="s">
-        <v>20</v>
-      </c>
-      <c r="W14" t="s">
         <v>48</v>
       </c>
-      <c r="X14">
+      <c r="W14">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>56</v>
       </c>
@@ -1468,21 +1452,17 @@
       <c r="S15">
         <v>1760</v>
       </c>
-      <c r="T15">
-        <f>SUM(S13:S15)</f>
-        <v>4160</v>
+      <c r="U15" t="s">
+        <v>20</v>
       </c>
       <c r="V15" t="s">
-        <v>20</v>
-      </c>
-      <c r="W15" t="s">
         <v>49</v>
       </c>
-      <c r="X15">
+      <c r="W15">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>50</v>
       </c>
@@ -1510,17 +1490,17 @@
       <c r="O16">
         <v>2</v>
       </c>
+      <c r="U16" t="s">
+        <v>20</v>
+      </c>
       <c r="V16" t="s">
-        <v>20</v>
-      </c>
-      <c r="W16" t="s">
         <v>56</v>
       </c>
-      <c r="X16">
+      <c r="W16">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>51</v>
       </c>
@@ -1548,17 +1528,17 @@
       <c r="O17">
         <v>4</v>
       </c>
+      <c r="U17" t="s">
+        <v>20</v>
+      </c>
       <c r="V17" t="s">
-        <v>20</v>
-      </c>
-      <c r="W17" t="s">
         <v>50</v>
       </c>
-      <c r="X17">
+      <c r="W17">
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>52</v>
       </c>
@@ -1586,17 +1566,17 @@
       <c r="O18">
         <v>4</v>
       </c>
+      <c r="U18" t="s">
+        <v>20</v>
+      </c>
       <c r="V18" t="s">
-        <v>20</v>
-      </c>
-      <c r="W18" t="s">
         <v>51</v>
       </c>
-      <c r="X18">
+      <c r="W18">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>53</v>
       </c>
@@ -1624,17 +1604,17 @@
       <c r="O19">
         <v>1</v>
       </c>
+      <c r="U19" t="s">
+        <v>20</v>
+      </c>
       <c r="V19" t="s">
-        <v>20</v>
-      </c>
-      <c r="W19" t="s">
         <v>52</v>
       </c>
-      <c r="X19">
+      <c r="W19">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>54</v>
       </c>
@@ -1662,17 +1642,17 @@
       <c r="O20">
         <v>2</v>
       </c>
+      <c r="U20" t="s">
+        <v>20</v>
+      </c>
       <c r="V20" t="s">
-        <v>20</v>
-      </c>
-      <c r="W20" t="s">
         <v>53</v>
       </c>
-      <c r="X20">
+      <c r="W20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:23" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>55</v>
       </c>
@@ -1700,17 +1680,17 @@
       <c r="O21">
         <v>4</v>
       </c>
+      <c r="U21" t="s">
+        <v>20</v>
+      </c>
       <c r="V21" t="s">
-        <v>20</v>
-      </c>
-      <c r="W21" t="s">
         <v>54</v>
       </c>
-      <c r="X21">
+      <c r="W21">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G22" t="s">
         <v>21</v>
       </c>
@@ -1735,21 +1715,17 @@
       <c r="O22">
         <v>3</v>
       </c>
+      <c r="U22" t="s">
+        <v>20</v>
+      </c>
       <c r="V22" t="s">
-        <v>20</v>
-      </c>
-      <c r="W22" t="s">
         <v>55</v>
       </c>
-      <c r="X22">
+      <c r="W22">
         <v>120</v>
       </c>
-      <c r="Y22">
-        <f>SUM(X3:X22)</f>
-        <v>2060</v>
-      </c>
-    </row>
-    <row r="23" spans="3:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G23" t="s">
         <v>21</v>
       </c>
@@ -1774,17 +1750,17 @@
       <c r="O23">
         <v>5</v>
       </c>
+      <c r="U23" t="s">
+        <v>21</v>
+      </c>
       <c r="V23" t="s">
-        <v>21</v>
-      </c>
-      <c r="W23" t="s">
         <v>15</v>
       </c>
-      <c r="X23">
+      <c r="W23">
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G24" t="s">
         <v>21</v>
       </c>
@@ -1809,17 +1785,17 @@
       <c r="O24">
         <v>6</v>
       </c>
+      <c r="U24" t="s">
+        <v>21</v>
+      </c>
       <c r="V24" t="s">
-        <v>21</v>
-      </c>
-      <c r="W24" t="s">
         <v>16</v>
       </c>
-      <c r="X24">
+      <c r="W24">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G25" t="s">
         <v>21</v>
       </c>
@@ -1844,17 +1820,17 @@
       <c r="O25">
         <v>5</v>
       </c>
+      <c r="U25" t="s">
+        <v>21</v>
+      </c>
       <c r="V25" t="s">
-        <v>21</v>
-      </c>
-      <c r="W25" t="s">
         <v>17</v>
       </c>
-      <c r="X25">
+      <c r="W25">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G26" t="s">
         <v>21</v>
       </c>
@@ -1879,17 +1855,17 @@
       <c r="O26">
         <v>7</v>
       </c>
+      <c r="U26" t="s">
+        <v>21</v>
+      </c>
       <c r="V26" t="s">
-        <v>21</v>
-      </c>
-      <c r="W26" t="s">
         <v>18</v>
       </c>
-      <c r="X26">
+      <c r="W26">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G27" t="s">
         <v>21</v>
       </c>
@@ -1914,17 +1890,17 @@
       <c r="O27">
         <v>2</v>
       </c>
+      <c r="U27" t="s">
+        <v>21</v>
+      </c>
       <c r="V27" t="s">
-        <v>21</v>
-      </c>
-      <c r="W27" t="s">
         <v>19</v>
       </c>
-      <c r="X27">
+      <c r="W27">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G28" t="s">
         <v>21</v>
       </c>
@@ -1949,17 +1925,17 @@
       <c r="O28">
         <v>2</v>
       </c>
+      <c r="U28" t="s">
+        <v>21</v>
+      </c>
       <c r="V28" t="s">
-        <v>21</v>
-      </c>
-      <c r="W28" t="s">
         <v>42</v>
       </c>
-      <c r="X28">
+      <c r="W28">
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G29" t="s">
         <v>21</v>
       </c>
@@ -1984,17 +1960,17 @@
       <c r="O29">
         <v>4</v>
       </c>
+      <c r="U29" t="s">
+        <v>21</v>
+      </c>
       <c r="V29" t="s">
-        <v>21</v>
-      </c>
-      <c r="W29" t="s">
         <v>43</v>
       </c>
-      <c r="X29">
+      <c r="W29">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
         <v>21</v>
       </c>
@@ -2019,17 +1995,17 @@
       <c r="O30">
         <v>3</v>
       </c>
+      <c r="U30" t="s">
+        <v>21</v>
+      </c>
       <c r="V30" t="s">
-        <v>21</v>
-      </c>
-      <c r="W30" t="s">
         <v>44</v>
       </c>
-      <c r="X30">
+      <c r="W30">
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G31" t="s">
         <v>28</v>
       </c>
@@ -2054,17 +2030,17 @@
       <c r="O31">
         <v>2</v>
       </c>
+      <c r="U31" t="s">
+        <v>21</v>
+      </c>
       <c r="V31" t="s">
-        <v>21</v>
-      </c>
-      <c r="W31" t="s">
         <v>45</v>
       </c>
-      <c r="X31">
+      <c r="W31">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:23" x14ac:dyDescent="0.2">
       <c r="G32" t="s">
         <v>28</v>
       </c>
@@ -2089,17 +2065,17 @@
       <c r="O32">
         <v>1</v>
       </c>
+      <c r="U32" t="s">
+        <v>21</v>
+      </c>
       <c r="V32" t="s">
-        <v>21</v>
-      </c>
-      <c r="W32" t="s">
         <v>47</v>
       </c>
-      <c r="X32">
+      <c r="W32">
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
         <v>28</v>
       </c>
@@ -2124,17 +2100,17 @@
       <c r="O33">
         <v>4</v>
       </c>
+      <c r="U33" t="s">
+        <v>21</v>
+      </c>
       <c r="V33" t="s">
-        <v>21</v>
-      </c>
-      <c r="W33" t="s">
         <v>46</v>
       </c>
-      <c r="X33">
+      <c r="W33">
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G34" t="s">
         <v>28</v>
       </c>
@@ -2159,17 +2135,17 @@
       <c r="O34">
         <v>4</v>
       </c>
+      <c r="U34" t="s">
+        <v>21</v>
+      </c>
       <c r="V34" t="s">
-        <v>21</v>
-      </c>
-      <c r="W34" t="s">
         <v>48</v>
       </c>
-      <c r="X34">
+      <c r="W34">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
         <v>28</v>
       </c>
@@ -2194,17 +2170,17 @@
       <c r="O35">
         <v>1</v>
       </c>
+      <c r="U35" t="s">
+        <v>21</v>
+      </c>
       <c r="V35" t="s">
-        <v>21</v>
-      </c>
-      <c r="W35" t="s">
         <v>49</v>
       </c>
-      <c r="X35">
+      <c r="W35">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="36" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G36" t="s">
         <v>28</v>
       </c>
@@ -2229,17 +2205,17 @@
       <c r="O36">
         <v>1</v>
       </c>
+      <c r="U36" t="s">
+        <v>21</v>
+      </c>
       <c r="V36" t="s">
-        <v>21</v>
-      </c>
-      <c r="W36" t="s">
         <v>56</v>
       </c>
-      <c r="X36">
+      <c r="W36">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
         <v>28</v>
       </c>
@@ -2264,17 +2240,17 @@
       <c r="O37">
         <v>4</v>
       </c>
+      <c r="U37" t="s">
+        <v>21</v>
+      </c>
       <c r="V37" t="s">
-        <v>21</v>
-      </c>
-      <c r="W37" t="s">
         <v>50</v>
       </c>
-      <c r="X37">
+      <c r="W37">
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G38" t="s">
         <v>28</v>
       </c>
@@ -2299,17 +2275,17 @@
       <c r="O38">
         <v>5</v>
       </c>
+      <c r="U38" t="s">
+        <v>21</v>
+      </c>
       <c r="V38" t="s">
-        <v>21</v>
-      </c>
-      <c r="W38" t="s">
         <v>51</v>
       </c>
-      <c r="X38">
+      <c r="W38">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G39" t="s">
         <v>28</v>
       </c>
@@ -2334,17 +2310,17 @@
       <c r="O39">
         <v>1</v>
       </c>
+      <c r="U39" t="s">
+        <v>21</v>
+      </c>
       <c r="V39" t="s">
-        <v>21</v>
-      </c>
-      <c r="W39" t="s">
         <v>52</v>
       </c>
-      <c r="X39">
+      <c r="W39">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G40" t="s">
         <v>28</v>
       </c>
@@ -2369,17 +2345,17 @@
       <c r="O40">
         <v>2</v>
       </c>
+      <c r="U40" t="s">
+        <v>21</v>
+      </c>
       <c r="V40" t="s">
-        <v>21</v>
-      </c>
-      <c r="W40" t="s">
         <v>53</v>
       </c>
-      <c r="X40">
+      <c r="W40">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G41" t="s">
         <v>28</v>
       </c>
@@ -2404,17 +2380,17 @@
       <c r="O41">
         <v>4</v>
       </c>
+      <c r="U41" t="s">
+        <v>21</v>
+      </c>
       <c r="V41" t="s">
-        <v>21</v>
-      </c>
-      <c r="W41" t="s">
         <v>54</v>
       </c>
-      <c r="X41">
+      <c r="W41">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="42" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G42" t="s">
         <v>28</v>
       </c>
@@ -2439,21 +2415,17 @@
       <c r="O42">
         <v>5</v>
       </c>
+      <c r="U42" t="s">
+        <v>21</v>
+      </c>
       <c r="V42" t="s">
-        <v>21</v>
-      </c>
-      <c r="W42" t="s">
         <v>55</v>
       </c>
-      <c r="X42">
+      <c r="W42">
         <v>130</v>
       </c>
-      <c r="Y42">
-        <f>SUM(X23:X42)</f>
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="43" spans="7:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G43" t="s">
         <v>29</v>
       </c>
@@ -2478,17 +2450,17 @@
       <c r="O43">
         <v>2</v>
       </c>
+      <c r="U43" t="s">
+        <v>28</v>
+      </c>
       <c r="V43" t="s">
-        <v>28</v>
-      </c>
-      <c r="W43" t="s">
         <v>15</v>
       </c>
-      <c r="X43">
+      <c r="W43">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G44" t="s">
         <v>29</v>
       </c>
@@ -2513,17 +2485,17 @@
       <c r="O44">
         <v>2</v>
       </c>
+      <c r="U44" t="s">
+        <v>28</v>
+      </c>
       <c r="V44" t="s">
-        <v>28</v>
-      </c>
-      <c r="W44" t="s">
         <v>16</v>
       </c>
-      <c r="X44">
+      <c r="W44">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G45" t="s">
         <v>29</v>
       </c>
@@ -2548,17 +2520,17 @@
       <c r="O45">
         <v>3</v>
       </c>
+      <c r="U45" t="s">
+        <v>28</v>
+      </c>
       <c r="V45" t="s">
-        <v>28</v>
-      </c>
-      <c r="W45" t="s">
         <v>17</v>
       </c>
-      <c r="X45">
+      <c r="W45">
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G46" t="s">
         <v>29</v>
       </c>
@@ -2583,17 +2555,17 @@
       <c r="O46">
         <v>4</v>
       </c>
+      <c r="U46" t="s">
+        <v>28</v>
+      </c>
       <c r="V46" t="s">
-        <v>28</v>
-      </c>
-      <c r="W46" t="s">
         <v>18</v>
       </c>
-      <c r="X46">
+      <c r="W46">
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G47" t="s">
         <v>29</v>
       </c>
@@ -2618,17 +2590,17 @@
       <c r="O47">
         <v>1</v>
       </c>
+      <c r="U47" t="s">
+        <v>28</v>
+      </c>
       <c r="V47" t="s">
-        <v>28</v>
-      </c>
-      <c r="W47" t="s">
         <v>19</v>
       </c>
-      <c r="X47">
+      <c r="W47">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G48" t="s">
         <v>29</v>
       </c>
@@ -2653,17 +2625,17 @@
       <c r="O48">
         <v>2</v>
       </c>
+      <c r="U48" t="s">
+        <v>28</v>
+      </c>
       <c r="V48" t="s">
-        <v>28</v>
-      </c>
-      <c r="W48" t="s">
         <v>42</v>
       </c>
-      <c r="X48">
+      <c r="W48">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G49" t="s">
         <v>29</v>
       </c>
@@ -2688,17 +2660,17 @@
       <c r="O49">
         <v>3</v>
       </c>
+      <c r="U49" t="s">
+        <v>28</v>
+      </c>
       <c r="V49" t="s">
-        <v>28</v>
-      </c>
-      <c r="W49" t="s">
         <v>43</v>
       </c>
-      <c r="X49">
+      <c r="W49">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G50" t="s">
         <v>29</v>
       </c>
@@ -2723,17 +2695,17 @@
       <c r="O50">
         <v>4</v>
       </c>
+      <c r="U50" t="s">
+        <v>28</v>
+      </c>
       <c r="V50" t="s">
-        <v>28</v>
-      </c>
-      <c r="W50" t="s">
         <v>44</v>
       </c>
-      <c r="X50">
+      <c r="W50">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G51" t="s">
         <v>29</v>
       </c>
@@ -2758,17 +2730,17 @@
       <c r="O51">
         <v>2</v>
       </c>
+      <c r="U51" t="s">
+        <v>28</v>
+      </c>
       <c r="V51" t="s">
-        <v>28</v>
-      </c>
-      <c r="W51" t="s">
         <v>45</v>
       </c>
-      <c r="X51">
+      <c r="W51">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="52" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G52" t="s">
         <v>29</v>
       </c>
@@ -2793,17 +2765,17 @@
       <c r="O52">
         <v>1</v>
       </c>
+      <c r="U52" t="s">
+        <v>28</v>
+      </c>
       <c r="V52" t="s">
-        <v>28</v>
-      </c>
-      <c r="W52" t="s">
         <v>47</v>
       </c>
-      <c r="X52">
+      <c r="W52">
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="53" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G53" t="s">
         <v>29</v>
       </c>
@@ -2828,17 +2800,17 @@
       <c r="O53">
         <v>3</v>
       </c>
+      <c r="U53" t="s">
+        <v>28</v>
+      </c>
       <c r="V53" t="s">
-        <v>28</v>
-      </c>
-      <c r="W53" t="s">
         <v>46</v>
       </c>
-      <c r="X53">
+      <c r="W53">
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="54" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G54" t="s">
         <v>29</v>
       </c>
@@ -2863,17 +2835,17 @@
       <c r="O54">
         <v>4</v>
       </c>
+      <c r="U54" t="s">
+        <v>28</v>
+      </c>
       <c r="V54" t="s">
-        <v>28</v>
-      </c>
-      <c r="W54" t="s">
         <v>48</v>
       </c>
-      <c r="X54">
+      <c r="W54">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="55" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G55" t="s">
         <v>29</v>
       </c>
@@ -2898,17 +2870,17 @@
       <c r="O55">
         <v>2</v>
       </c>
+      <c r="U55" t="s">
+        <v>28</v>
+      </c>
       <c r="V55" t="s">
-        <v>28</v>
-      </c>
-      <c r="W55" t="s">
         <v>49</v>
       </c>
-      <c r="X55">
+      <c r="W55">
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G56" t="s">
         <v>35</v>
       </c>
@@ -2933,17 +2905,17 @@
       <c r="O56">
         <v>2</v>
       </c>
+      <c r="U56" t="s">
+        <v>28</v>
+      </c>
       <c r="V56" t="s">
-        <v>28</v>
-      </c>
-      <c r="W56" t="s">
         <v>56</v>
       </c>
-      <c r="X56">
+      <c r="W56">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G57" t="s">
         <v>35</v>
       </c>
@@ -2968,17 +2940,17 @@
       <c r="O57">
         <v>4</v>
       </c>
+      <c r="U57" t="s">
+        <v>28</v>
+      </c>
       <c r="V57" t="s">
-        <v>28</v>
-      </c>
-      <c r="W57" t="s">
         <v>50</v>
       </c>
-      <c r="X57">
+      <c r="W57">
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="58" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G58" t="s">
         <v>35</v>
       </c>
@@ -3003,17 +2975,17 @@
       <c r="O58">
         <v>4</v>
       </c>
+      <c r="U58" t="s">
+        <v>28</v>
+      </c>
       <c r="V58" t="s">
-        <v>28</v>
-      </c>
-      <c r="W58" t="s">
         <v>51</v>
       </c>
-      <c r="X58">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="7:25" x14ac:dyDescent="0.2">
+      <c r="W58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G59" t="s">
         <v>35</v>
       </c>
@@ -3038,17 +3010,17 @@
       <c r="O59">
         <v>1</v>
       </c>
+      <c r="U59" t="s">
+        <v>28</v>
+      </c>
       <c r="V59" t="s">
-        <v>28</v>
-      </c>
-      <c r="W59" t="s">
         <v>52</v>
       </c>
-      <c r="X59">
+      <c r="W59">
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="60" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G60" t="s">
         <v>35</v>
       </c>
@@ -3073,17 +3045,17 @@
       <c r="O60">
         <v>2</v>
       </c>
+      <c r="U60" t="s">
+        <v>28</v>
+      </c>
       <c r="V60" t="s">
-        <v>28</v>
-      </c>
-      <c r="W60" t="s">
         <v>53</v>
       </c>
-      <c r="X60">
+      <c r="W60">
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G61" t="s">
         <v>35</v>
       </c>
@@ -3108,17 +3080,17 @@
       <c r="O61">
         <v>4</v>
       </c>
+      <c r="U61" t="s">
+        <v>28</v>
+      </c>
       <c r="V61" t="s">
-        <v>28</v>
-      </c>
-      <c r="W61" t="s">
         <v>54</v>
       </c>
-      <c r="X61">
+      <c r="W61">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G62" t="s">
         <v>35</v>
       </c>
@@ -3143,21 +3115,17 @@
       <c r="O62">
         <v>3</v>
       </c>
+      <c r="U62" t="s">
+        <v>28</v>
+      </c>
       <c r="V62" t="s">
-        <v>28</v>
-      </c>
-      <c r="W62" t="s">
         <v>55</v>
       </c>
-      <c r="X62">
+      <c r="W62">
         <v>70</v>
       </c>
-      <c r="Y62">
-        <f>SUM(X43:X62)</f>
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="63" spans="7:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G63" t="s">
         <v>35</v>
       </c>
@@ -3182,17 +3150,17 @@
       <c r="O63">
         <v>5</v>
       </c>
+      <c r="U63" t="s">
+        <v>29</v>
+      </c>
       <c r="V63" t="s">
-        <v>29</v>
-      </c>
-      <c r="W63" t="s">
         <v>15</v>
       </c>
-      <c r="X63">
+      <c r="W63">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="7:25" x14ac:dyDescent="0.2">
+    <row r="64" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G64" t="s">
         <v>35</v>
       </c>
@@ -3217,17 +3185,17 @@
       <c r="O64">
         <v>6</v>
       </c>
+      <c r="U64" t="s">
+        <v>29</v>
+      </c>
       <c r="V64" t="s">
-        <v>29</v>
-      </c>
-      <c r="W64" t="s">
         <v>16</v>
       </c>
-      <c r="X64">
+      <c r="W64">
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="7:24" x14ac:dyDescent="0.2">
+    <row r="65" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G65" t="s">
         <v>35</v>
       </c>
@@ -3252,17 +3220,17 @@
       <c r="O65">
         <v>5</v>
       </c>
+      <c r="U65" t="s">
+        <v>29</v>
+      </c>
       <c r="V65" t="s">
-        <v>29</v>
-      </c>
-      <c r="W65" t="s">
         <v>17</v>
       </c>
-      <c r="X65">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="7:24" x14ac:dyDescent="0.2">
+      <c r="W65">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G66" t="s">
         <v>35</v>
       </c>
@@ -3287,17 +3255,17 @@
       <c r="O66">
         <v>7</v>
       </c>
+      <c r="U66" t="s">
+        <v>29</v>
+      </c>
       <c r="V66" t="s">
-        <v>29</v>
-      </c>
-      <c r="W66" t="s">
         <v>18</v>
       </c>
-      <c r="X66">
+      <c r="W66">
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="7:24" x14ac:dyDescent="0.2">
+    <row r="67" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G67" t="s">
         <v>35</v>
       </c>
@@ -3322,17 +3290,17 @@
       <c r="O67">
         <v>2</v>
       </c>
+      <c r="U67" t="s">
+        <v>29</v>
+      </c>
       <c r="V67" t="s">
-        <v>29</v>
-      </c>
-      <c r="W67" t="s">
         <v>19</v>
       </c>
-      <c r="X67">
+      <c r="W67">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="7:24" x14ac:dyDescent="0.2">
+    <row r="68" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G68" t="s">
         <v>35</v>
       </c>
@@ -3357,17 +3325,17 @@
       <c r="O68">
         <v>2</v>
       </c>
+      <c r="U68" t="s">
+        <v>29</v>
+      </c>
       <c r="V68" t="s">
-        <v>29</v>
-      </c>
-      <c r="W68" t="s">
         <v>42</v>
       </c>
-      <c r="X68">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" spans="7:24" x14ac:dyDescent="0.2">
+      <c r="W68">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G69" t="s">
         <v>35</v>
       </c>
@@ -3392,17 +3360,17 @@
       <c r="O69">
         <v>4</v>
       </c>
+      <c r="U69" t="s">
+        <v>29</v>
+      </c>
       <c r="V69" t="s">
-        <v>29</v>
-      </c>
-      <c r="W69" t="s">
         <v>43</v>
       </c>
-      <c r="X69">
+      <c r="W69">
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="7:24" x14ac:dyDescent="0.2">
+    <row r="70" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G70" t="s">
         <v>35</v>
       </c>
@@ -3427,17 +3395,17 @@
       <c r="O70">
         <v>3</v>
       </c>
+      <c r="U70" t="s">
+        <v>29</v>
+      </c>
       <c r="V70" t="s">
-        <v>29</v>
-      </c>
-      <c r="W70" t="s">
         <v>44</v>
       </c>
-      <c r="X70">
+      <c r="W70">
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="7:24" x14ac:dyDescent="0.2">
+    <row r="71" spans="7:23" x14ac:dyDescent="0.2">
       <c r="G71" t="s">
         <v>35</v>
       </c>
@@ -3462,17 +3430,17 @@
       <c r="O71">
         <v>2</v>
       </c>
+      <c r="U71" t="s">
+        <v>29</v>
+      </c>
       <c r="V71" t="s">
-        <v>29</v>
-      </c>
-      <c r="W71" t="s">
         <v>45</v>
       </c>
-      <c r="X71">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="72" spans="7:24" x14ac:dyDescent="0.2">
+      <c r="W71">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="7:23" x14ac:dyDescent="0.2">
       <c r="L72" t="s">
         <v>21</v>
       </c>
@@ -3485,17 +3453,17 @@
       <c r="O72">
         <v>1</v>
       </c>
+      <c r="U72" t="s">
+        <v>29</v>
+      </c>
       <c r="V72" t="s">
-        <v>29</v>
-      </c>
-      <c r="W72" t="s">
         <v>47</v>
       </c>
-      <c r="X72">
+      <c r="W72">
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="7:24" x14ac:dyDescent="0.2">
+    <row r="73" spans="7:23" x14ac:dyDescent="0.2">
       <c r="L73" t="s">
         <v>21</v>
       </c>
@@ -3508,17 +3476,17 @@
       <c r="O73">
         <v>4</v>
       </c>
+      <c r="U73" t="s">
+        <v>29</v>
+      </c>
       <c r="V73" t="s">
-        <v>29</v>
-      </c>
-      <c r="W73" t="s">
         <v>46</v>
       </c>
-      <c r="X73">
+      <c r="W73">
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="7:24" x14ac:dyDescent="0.2">
+    <row r="74" spans="7:23" x14ac:dyDescent="0.2">
       <c r="L74" t="s">
         <v>21</v>
       </c>
@@ -3531,17 +3499,17 @@
       <c r="O74">
         <v>4</v>
       </c>
+      <c r="U74" t="s">
+        <v>29</v>
+      </c>
       <c r="V74" t="s">
-        <v>29</v>
-      </c>
-      <c r="W74" t="s">
         <v>48</v>
       </c>
-      <c r="X74">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="75" spans="7:24" x14ac:dyDescent="0.2">
+      <c r="W74">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="7:23" x14ac:dyDescent="0.2">
       <c r="L75" t="s">
         <v>21</v>
       </c>
@@ -3554,17 +3522,17 @@
       <c r="O75">
         <v>1</v>
       </c>
+      <c r="U75" t="s">
+        <v>29</v>
+      </c>
       <c r="V75" t="s">
-        <v>29</v>
-      </c>
-      <c r="W75" t="s">
         <v>49</v>
       </c>
-      <c r="X75">
+      <c r="W75">
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="7:24" x14ac:dyDescent="0.2">
+    <row r="76" spans="7:23" x14ac:dyDescent="0.2">
       <c r="L76" t="s">
         <v>21</v>
       </c>
@@ -3577,17 +3545,17 @@
       <c r="O76">
         <v>1</v>
       </c>
+      <c r="U76" t="s">
+        <v>29</v>
+      </c>
       <c r="V76" t="s">
-        <v>29</v>
-      </c>
-      <c r="W76" t="s">
         <v>56</v>
       </c>
-      <c r="X76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="77" spans="7:24" x14ac:dyDescent="0.2">
+      <c r="W76">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="7:23" x14ac:dyDescent="0.2">
       <c r="L77" t="s">
         <v>21</v>
       </c>
@@ -3600,17 +3568,17 @@
       <c r="O77">
         <v>4</v>
       </c>
+      <c r="U77" t="s">
+        <v>29</v>
+      </c>
       <c r="V77" t="s">
-        <v>29</v>
-      </c>
-      <c r="W77" t="s">
         <v>50</v>
       </c>
-      <c r="X77">
+      <c r="W77">
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="7:24" x14ac:dyDescent="0.2">
+    <row r="78" spans="7:23" x14ac:dyDescent="0.2">
       <c r="L78" t="s">
         <v>21</v>
       </c>
@@ -3623,17 +3591,17 @@
       <c r="O78">
         <v>5</v>
       </c>
+      <c r="U78" t="s">
+        <v>29</v>
+      </c>
       <c r="V78" t="s">
-        <v>29</v>
-      </c>
-      <c r="W78" t="s">
         <v>51</v>
       </c>
-      <c r="X78">
+      <c r="W78">
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="7:24" x14ac:dyDescent="0.2">
+    <row r="79" spans="7:23" x14ac:dyDescent="0.2">
       <c r="L79" t="s">
         <v>21</v>
       </c>
@@ -3646,17 +3614,17 @@
       <c r="O79">
         <v>1</v>
       </c>
+      <c r="U79" t="s">
+        <v>29</v>
+      </c>
       <c r="V79" t="s">
-        <v>29</v>
-      </c>
-      <c r="W79" t="s">
         <v>52</v>
       </c>
-      <c r="X79">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" spans="7:24" x14ac:dyDescent="0.2">
+      <c r="W79">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="7:23" x14ac:dyDescent="0.2">
       <c r="L80" t="s">
         <v>21</v>
       </c>
@@ -3669,17 +3637,17 @@
       <c r="O80">
         <v>2</v>
       </c>
+      <c r="U80" t="s">
+        <v>29</v>
+      </c>
       <c r="V80" t="s">
-        <v>29</v>
-      </c>
-      <c r="W80" t="s">
         <v>53</v>
       </c>
-      <c r="X80">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="81" spans="12:25" x14ac:dyDescent="0.2">
+      <c r="W80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L81" t="s">
         <v>21</v>
       </c>
@@ -3692,17 +3660,17 @@
       <c r="O81">
         <v>4</v>
       </c>
+      <c r="U81" t="s">
+        <v>29</v>
+      </c>
       <c r="V81" t="s">
-        <v>29</v>
-      </c>
-      <c r="W81" t="s">
         <v>54</v>
       </c>
-      <c r="X81">
+      <c r="W81">
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="82" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L82" t="s">
         <v>21</v>
       </c>
@@ -3715,21 +3683,17 @@
       <c r="O82">
         <v>5</v>
       </c>
+      <c r="U82" t="s">
+        <v>29</v>
+      </c>
       <c r="V82" t="s">
-        <v>29</v>
-      </c>
-      <c r="W82" t="s">
         <v>55</v>
       </c>
-      <c r="X82">
+      <c r="W82">
         <v>60</v>
       </c>
-      <c r="Y82">
-        <f>SUM(X63:X82)</f>
-        <v>580</v>
-      </c>
-    </row>
-    <row r="83" spans="12:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L83" t="s">
         <v>28</v>
       </c>
@@ -3742,17 +3706,17 @@
       <c r="O83" s="1">
         <v>2</v>
       </c>
+      <c r="U83" t="s">
+        <v>35</v>
+      </c>
       <c r="V83" t="s">
-        <v>35</v>
-      </c>
-      <c r="W83" t="s">
         <v>15</v>
       </c>
-      <c r="X83">
+      <c r="W83">
         <v>300</v>
       </c>
     </row>
-    <row r="84" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="84" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L84" t="s">
         <v>28</v>
       </c>
@@ -3765,17 +3729,17 @@
       <c r="O84" s="1">
         <v>2</v>
       </c>
+      <c r="U84" t="s">
+        <v>35</v>
+      </c>
       <c r="V84" t="s">
-        <v>35</v>
-      </c>
-      <c r="W84" t="s">
         <v>16</v>
       </c>
-      <c r="X84">
+      <c r="W84">
         <v>200</v>
       </c>
     </row>
-    <row r="85" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="85" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L85" t="s">
         <v>28</v>
       </c>
@@ -3788,17 +3752,17 @@
       <c r="O85" s="1">
         <v>3</v>
       </c>
+      <c r="U85" t="s">
+        <v>35</v>
+      </c>
       <c r="V85" t="s">
-        <v>35</v>
-      </c>
-      <c r="W85" t="s">
         <v>17</v>
       </c>
-      <c r="X85">
+      <c r="W85">
         <v>150</v>
       </c>
     </row>
-    <row r="86" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="86" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L86" t="s">
         <v>28</v>
       </c>
@@ -3811,17 +3775,17 @@
       <c r="O86" s="1">
         <v>4</v>
       </c>
+      <c r="U86" t="s">
+        <v>35</v>
+      </c>
       <c r="V86" t="s">
-        <v>35</v>
-      </c>
-      <c r="W86" t="s">
         <v>18</v>
       </c>
-      <c r="X86">
+      <c r="W86">
         <v>300</v>
       </c>
     </row>
-    <row r="87" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="87" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L87" t="s">
         <v>28</v>
       </c>
@@ -3834,17 +3798,17 @@
       <c r="O87" s="1">
         <v>1</v>
       </c>
+      <c r="U87" t="s">
+        <v>35</v>
+      </c>
       <c r="V87" t="s">
-        <v>35</v>
-      </c>
-      <c r="W87" t="s">
         <v>19</v>
       </c>
-      <c r="X87">
+      <c r="W87">
         <v>140</v>
       </c>
     </row>
-    <row r="88" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="88" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L88" t="s">
         <v>28</v>
       </c>
@@ -3857,17 +3821,17 @@
       <c r="O88" s="1">
         <v>2</v>
       </c>
+      <c r="U88" t="s">
+        <v>35</v>
+      </c>
       <c r="V88" t="s">
-        <v>35</v>
-      </c>
-      <c r="W88" t="s">
         <v>42</v>
       </c>
-      <c r="X88">
+      <c r="W88">
         <v>150</v>
       </c>
     </row>
-    <row r="89" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="89" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L89" t="s">
         <v>28</v>
       </c>
@@ -3880,17 +3844,17 @@
       <c r="O89" s="1">
         <v>3</v>
       </c>
+      <c r="U89" t="s">
+        <v>35</v>
+      </c>
       <c r="V89" t="s">
-        <v>35</v>
-      </c>
-      <c r="W89" t="s">
         <v>43</v>
       </c>
-      <c r="X89">
+      <c r="W89">
         <v>240</v>
       </c>
     </row>
-    <row r="90" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="90" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L90" t="s">
         <v>28</v>
       </c>
@@ -3903,17 +3867,17 @@
       <c r="O90" s="1">
         <v>4</v>
       </c>
+      <c r="U90" t="s">
+        <v>35</v>
+      </c>
       <c r="V90" t="s">
-        <v>35</v>
-      </c>
-      <c r="W90" t="s">
         <v>44</v>
       </c>
-      <c r="X90">
+      <c r="W90">
         <v>210</v>
       </c>
     </row>
-    <row r="91" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="91" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L91" t="s">
         <v>28</v>
       </c>
@@ -3926,17 +3890,17 @@
       <c r="O91" s="1">
         <v>2</v>
       </c>
+      <c r="U91" t="s">
+        <v>35</v>
+      </c>
       <c r="V91" t="s">
-        <v>35</v>
-      </c>
-      <c r="W91" t="s">
         <v>45</v>
       </c>
-      <c r="X91">
+      <c r="W91">
         <v>180</v>
       </c>
     </row>
-    <row r="92" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="92" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L92" t="s">
         <v>28</v>
       </c>
@@ -3949,17 +3913,17 @@
       <c r="O92" s="1">
         <v>1</v>
       </c>
+      <c r="U92" t="s">
+        <v>35</v>
+      </c>
       <c r="V92" t="s">
-        <v>35</v>
-      </c>
-      <c r="W92" t="s">
         <v>47</v>
       </c>
-      <c r="X92">
+      <c r="W92">
         <v>390</v>
       </c>
     </row>
-    <row r="93" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="93" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L93" t="s">
         <v>28</v>
       </c>
@@ -3972,17 +3936,17 @@
       <c r="O93" s="1">
         <v>3</v>
       </c>
+      <c r="U93" t="s">
+        <v>35</v>
+      </c>
       <c r="V93" t="s">
-        <v>35</v>
-      </c>
-      <c r="W93" t="s">
         <v>46</v>
       </c>
-      <c r="X93">
+      <c r="W93">
         <v>360</v>
       </c>
     </row>
-    <row r="94" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="94" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L94" t="s">
         <v>28</v>
       </c>
@@ -3995,17 +3959,17 @@
       <c r="O94" s="1">
         <v>4</v>
       </c>
+      <c r="U94" t="s">
+        <v>35</v>
+      </c>
       <c r="V94" t="s">
-        <v>35</v>
-      </c>
-      <c r="W94" t="s">
         <v>48</v>
       </c>
-      <c r="X94">
+      <c r="W94">
         <v>150</v>
       </c>
     </row>
-    <row r="95" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="95" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L95" t="s">
         <v>28</v>
       </c>
@@ -4018,17 +3982,17 @@
       <c r="O95" s="1">
         <v>2</v>
       </c>
+      <c r="U95" t="s">
+        <v>35</v>
+      </c>
       <c r="V95" t="s">
-        <v>35</v>
-      </c>
-      <c r="W95" t="s">
         <v>49</v>
       </c>
-      <c r="X95">
+      <c r="W95">
         <v>140</v>
       </c>
     </row>
-    <row r="96" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="96" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L96" t="s">
         <v>28</v>
       </c>
@@ -4041,17 +4005,17 @@
       <c r="O96" s="1">
         <v>2</v>
       </c>
+      <c r="U96" t="s">
+        <v>35</v>
+      </c>
       <c r="V96" t="s">
-        <v>35</v>
-      </c>
-      <c r="W96" t="s">
         <v>56</v>
       </c>
-      <c r="X96">
+      <c r="W96">
         <v>200</v>
       </c>
     </row>
-    <row r="97" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="97" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L97" t="s">
         <v>28</v>
       </c>
@@ -4064,17 +4028,17 @@
       <c r="O97" s="1">
         <v>4</v>
       </c>
+      <c r="U97" t="s">
+        <v>35</v>
+      </c>
       <c r="V97" t="s">
-        <v>35</v>
-      </c>
-      <c r="W97" t="s">
         <v>50</v>
       </c>
-      <c r="X97">
+      <c r="W97">
         <v>250</v>
       </c>
     </row>
-    <row r="98" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="98" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L98" t="s">
         <v>28</v>
       </c>
@@ -4087,17 +4051,17 @@
       <c r="O98" s="1">
         <v>4</v>
       </c>
+      <c r="U98" t="s">
+        <v>35</v>
+      </c>
       <c r="V98" t="s">
-        <v>35</v>
-      </c>
-      <c r="W98" t="s">
         <v>51</v>
       </c>
-      <c r="X98">
+      <c r="W98">
         <v>130</v>
       </c>
     </row>
-    <row r="99" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="99" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L99" t="s">
         <v>28</v>
       </c>
@@ -4110,17 +4074,17 @@
       <c r="O99" s="1">
         <v>1</v>
       </c>
+      <c r="U99" t="s">
+        <v>35</v>
+      </c>
       <c r="V99" t="s">
-        <v>35</v>
-      </c>
-      <c r="W99" t="s">
         <v>52</v>
       </c>
-      <c r="X99">
+      <c r="W99">
         <v>130</v>
       </c>
     </row>
-    <row r="100" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="100" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L100" t="s">
         <v>28</v>
       </c>
@@ -4133,17 +4097,17 @@
       <c r="O100" s="1">
         <v>2</v>
       </c>
+      <c r="U100" t="s">
+        <v>35</v>
+      </c>
       <c r="V100" t="s">
-        <v>35</v>
-      </c>
-      <c r="W100" t="s">
         <v>53</v>
       </c>
-      <c r="X100">
+      <c r="W100">
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="101" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L101" t="s">
         <v>28</v>
       </c>
@@ -4156,17 +4120,17 @@
       <c r="O101" s="1">
         <v>4</v>
       </c>
+      <c r="U101" t="s">
+        <v>35</v>
+      </c>
       <c r="V101" t="s">
-        <v>35</v>
-      </c>
-      <c r="W101" t="s">
         <v>54</v>
       </c>
-      <c r="X101">
+      <c r="W101">
         <v>210</v>
       </c>
     </row>
-    <row r="102" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="102" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L102" t="s">
         <v>28</v>
       </c>
@@ -4179,21 +4143,17 @@
       <c r="O102" s="1">
         <v>3</v>
       </c>
+      <c r="U102" t="s">
+        <v>35</v>
+      </c>
       <c r="V102" t="s">
-        <v>35</v>
-      </c>
-      <c r="W102" t="s">
         <v>55</v>
       </c>
-      <c r="X102">
+      <c r="W102">
         <v>230</v>
       </c>
-      <c r="Y102">
-        <f>SUM(X83:X102)</f>
-        <v>4160</v>
-      </c>
-    </row>
-    <row r="103" spans="12:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L103" t="s">
         <v>28</v>
       </c>
@@ -4207,7 +4167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="104" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L104" t="s">
         <v>28</v>
       </c>
@@ -4221,7 +4181,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="105" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L105" t="s">
         <v>28</v>
       </c>
@@ -4235,7 +4195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="106" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L106" t="s">
         <v>28</v>
       </c>
@@ -4249,7 +4209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="107" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L107" t="s">
         <v>28</v>
       </c>
@@ -4263,7 +4223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="108" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L108" t="s">
         <v>28</v>
       </c>
@@ -4277,7 +4237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="109" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L109" t="s">
         <v>28</v>
       </c>
@@ -4291,7 +4251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="110" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L110" t="s">
         <v>28</v>
       </c>
@@ -4305,7 +4265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="111" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L111" t="s">
         <v>28</v>
       </c>
@@ -4319,7 +4279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="12:25" x14ac:dyDescent="0.2">
+    <row r="112" spans="12:23" x14ac:dyDescent="0.2">
       <c r="L112" t="s">
         <v>28</v>
       </c>

</xml_diff>